<commit_message>
If statements added to grammar
</commit_message>
<xml_diff>
--- a/src/SyntacticAnalyzer/Grammar.xlsx
+++ b/src/SyntacticAnalyzer/Grammar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\General\Trabajos\ProgrammingLanguages\src\SyntacticAnalyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E57AFC-2429-44F1-A3B5-DEE0E8EA2451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D938865-C45D-44AC-B807-623450C5EBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="87">
   <si>
     <t>S</t>
   </si>
@@ -738,6 +738,118 @@
         <scheme val="minor"/>
       </rPr>
       <t>token_cor_der</t>
+    </r>
+  </si>
+  <si>
+    <t>If</t>
+  </si>
+  <si>
+    <t>BooleanExpression</t>
+  </si>
+  <si>
+    <t>BooleanExpressionOp</t>
+  </si>
+  <si>
+    <t>BooleanBinaryOp</t>
+  </si>
+  <si>
+    <t>BooleanUnaryOp</t>
+  </si>
+  <si>
+    <t>token_dif</t>
+  </si>
+  <si>
+    <t>token_menor_igual</t>
+  </si>
+  <si>
+    <t>token_menor</t>
+  </si>
+  <si>
+    <t>token_mayor</t>
+  </si>
+  <si>
+    <t>token_mayor_igual</t>
+  </si>
+  <si>
+    <t>Else</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sino </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ProcessBody</t>
+    </r>
+  </si>
+  <si>
+    <t>ElseIf</t>
+  </si>
+  <si>
+    <t>Expression BooleanExpressionOp</t>
+  </si>
+  <si>
+    <t>BooleanBinaryOp BooleanExpression BooleanExpressionOp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>si</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> BooleanExpression </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>entonces</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ProcessBody ElseIf </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>finsi</t>
     </r>
   </si>
 </sst>
@@ -887,7 +999,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1070,12 +1182,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1240,17 +1346,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1606,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C105"/>
+  <dimension ref="B2:C123"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,10 +1746,10 @@
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1681,448 +1785,570 @@
         <v>15</v>
       </c>
     </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
+    </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C27" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C41" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" s="3"/>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="5"/>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" t="s">
-        <v>53</v>
+        <v>60</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" t="s">
-        <v>52</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C47" s="1"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" t="s">
-        <v>50</v>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>67</v>
-      </c>
-      <c r="C50" t="s">
-        <v>61</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C50" s="1"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>68</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>63</v>
-      </c>
+      <c r="C51" s="1"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>68</v>
+        <v>54</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>49</v>
-      </c>
-      <c r="C54" t="s">
-        <v>51</v>
+        <v>55</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>48</v>
+      </c>
+      <c r="C65" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>67</v>
+      </c>
+      <c r="C67" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>68</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="5" t="s">
+      <c r="C71" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C74" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="5" t="s">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C75" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="5" t="s">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C76" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="5" t="s">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C77" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="5" t="s">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C78" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="5" t="s">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C79" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="5" t="s">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C80" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="5" t="s">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C82" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="5" t="s">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C65" s="5"/>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+      <c r="C83" s="3"/>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C84" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="3" t="s">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="3" t="s">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="3" t="s">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C71" s="3"/>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="C89" s="3"/>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
         <v>18</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>18</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="5" t="s">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C94" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="5" t="s">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C95" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="5" t="s">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C96" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="5" t="s">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C97" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="5" t="s">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C98" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="5" t="s">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C99" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C92" s="2"/>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C93" s="2"/>
-    </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C105" s="1"/>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="2"/>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C111" s="2"/>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>